<commit_message>
questions for analyses and cleaning up data
</commit_message>
<xml_diff>
--- a/corridor_docs/eric_ms_thesis/ms_data/vial_labels.xlsx
+++ b/corridor_docs/eric_ms_thesis/ms_data/vial_labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericescobar-chena/corridor_thesis/corridor_docs/eric_ms_thesis/ms_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF16F145-1CD3-F242-B675-6846F411694E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A306D266-4A84-8F4C-AA92-936367B97187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16460" xr2:uid="{057DED21-1AFB-FA4C-B6FB-91551634657C}"/>
+    <workbookView xWindow="800" yWindow="500" windowWidth="28000" windowHeight="16460" xr2:uid="{057DED21-1AFB-FA4C-B6FB-91551634657C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="18" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29" defaultRowHeight="199" customHeight="1"/>
@@ -437,661 +437,701 @@
   <sheetData>
     <row r="1" spans="1:12" ht="199" customHeight="1">
       <c r="A1" s="1">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1">
-        <v>157</v>
+        <f>+A1</f>
+        <v>133</v>
       </c>
       <c r="C1" s="1">
-        <v>157</v>
+        <f t="shared" ref="C1:F1" si="0">+B1</f>
+        <v>133</v>
       </c>
       <c r="D1" s="1">
-        <v>157</v>
+        <f t="shared" si="0"/>
+        <v>133</v>
       </c>
       <c r="E1" s="1">
-        <v>157</v>
+        <f t="shared" si="0"/>
+        <v>133</v>
       </c>
       <c r="F1" s="1">
-        <v>157</v>
+        <f t="shared" si="0"/>
+        <v>133</v>
       </c>
       <c r="G1" s="1">
         <f>A1+1</f>
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1">
-        <f t="shared" ref="H1:L1" si="0">B1+1</f>
-        <v>158</v>
+        <f t="shared" ref="H1:L1" si="1">B1+1</f>
+        <v>134</v>
       </c>
       <c r="I1" s="1">
-        <f t="shared" si="0"/>
-        <v>158</v>
+        <f t="shared" si="1"/>
+        <v>134</v>
       </c>
       <c r="J1" s="1">
-        <f t="shared" si="0"/>
-        <v>158</v>
+        <f t="shared" si="1"/>
+        <v>134</v>
       </c>
       <c r="K1" s="1">
-        <f t="shared" si="0"/>
-        <v>158</v>
+        <f t="shared" si="1"/>
+        <v>134</v>
       </c>
       <c r="L1" s="1">
-        <f t="shared" si="0"/>
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="199" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="199" hidden="1" customHeight="1">
       <c r="A2" s="1">
         <f>A1+2</f>
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B2" s="1">
-        <f t="shared" ref="B2:F2" si="1">B1+2</f>
-        <v>159</v>
+        <f t="shared" ref="B2:F2" si="2">B1+2</f>
+        <v>135</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" si="1"/>
-        <v>159</v>
+        <f t="shared" si="2"/>
+        <v>135</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" si="1"/>
-        <v>159</v>
+        <f t="shared" si="2"/>
+        <v>135</v>
       </c>
       <c r="E2" s="1">
-        <f t="shared" si="1"/>
-        <v>159</v>
+        <f t="shared" si="2"/>
+        <v>135</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" si="1"/>
-        <v>159</v>
+        <f t="shared" si="2"/>
+        <v>135</v>
       </c>
       <c r="G2" s="1">
         <f>A1+3</f>
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" ref="H2:L2" si="2">B1+3</f>
-        <v>160</v>
+        <f t="shared" ref="H2:L2" si="3">B1+3</f>
+        <v>136</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" si="2"/>
-        <v>160</v>
+        <f t="shared" si="3"/>
+        <v>136</v>
       </c>
       <c r="J2" s="1">
-        <f t="shared" si="2"/>
-        <v>160</v>
+        <f t="shared" si="3"/>
+        <v>136</v>
       </c>
       <c r="K2" s="1">
-        <f t="shared" si="2"/>
-        <v>160</v>
+        <f t="shared" si="3"/>
+        <v>136</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" si="2"/>
-        <v>160</v>
+        <f t="shared" si="3"/>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="199" customHeight="1">
       <c r="A3" s="1">
-        <f>A1+4</f>
-        <v>161</v>
+        <f t="shared" ref="A3:E3" si="4">A1+2</f>
+        <v>135</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:F3" si="3">B1+4</f>
-        <v>161</v>
+        <f t="shared" si="4"/>
+        <v>135</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" si="3"/>
-        <v>161</v>
+        <f t="shared" si="4"/>
+        <v>135</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" si="3"/>
-        <v>161</v>
+        <f t="shared" si="4"/>
+        <v>135</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" si="3"/>
-        <v>161</v>
+        <f t="shared" si="4"/>
+        <v>135</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" si="3"/>
-        <v>161</v>
+        <f>F1+2</f>
+        <v>135</v>
       </c>
       <c r="G3" s="1">
-        <f>A1+5</f>
-        <v>162</v>
+        <f>A1+3</f>
+        <v>136</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:L3" si="4">B1+5</f>
-        <v>162</v>
+        <f>B1+3</f>
+        <v>136</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" si="4"/>
-        <v>162</v>
+        <f t="shared" ref="I3:L3" si="5">C1+3</f>
+        <v>136</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" si="4"/>
-        <v>162</v>
+        <f t="shared" si="5"/>
+        <v>136</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" si="4"/>
-        <v>162</v>
+        <f t="shared" si="5"/>
+        <v>136</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" si="4"/>
-        <v>162</v>
+        <f t="shared" si="5"/>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="199" customHeight="1">
       <c r="A4" s="1">
-        <f>A1+6</f>
-        <v>163</v>
+        <f t="shared" ref="A4:B4" si="6">A1+4</f>
+        <v>137</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:F4" si="5">B1+6</f>
-        <v>163</v>
+        <f t="shared" si="6"/>
+        <v>137</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="5"/>
-        <v>163</v>
+        <f>C1+4</f>
+        <v>137</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="5"/>
-        <v>163</v>
+        <f t="shared" ref="D4:F4" si="7">D1+4</f>
+        <v>137</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="5"/>
-        <v>163</v>
+        <f t="shared" si="7"/>
+        <v>137</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="5"/>
-        <v>163</v>
+        <f t="shared" si="7"/>
+        <v>137</v>
       </c>
       <c r="G4" s="1">
-        <f>A1+7</f>
-        <v>164</v>
+        <f>A1+5</f>
+        <v>138</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:L4" si="6">B1+7</f>
-        <v>164</v>
+        <f t="shared" ref="H4:L4" si="8">B1+5</f>
+        <v>138</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="6"/>
-        <v>164</v>
+        <f t="shared" si="8"/>
+        <v>138</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" si="6"/>
-        <v>164</v>
+        <f t="shared" si="8"/>
+        <v>138</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" si="6"/>
-        <v>164</v>
+        <f t="shared" si="8"/>
+        <v>138</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="6"/>
-        <v>164</v>
+        <f t="shared" si="8"/>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="199" customHeight="1">
       <c r="A5" s="1">
-        <f>A1+8</f>
-        <v>165</v>
+        <f>A1+6</f>
+        <v>139</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" ref="B5:F5" si="7">B1+8</f>
-        <v>165</v>
+        <f t="shared" ref="B5:F5" si="9">B1+6</f>
+        <v>139</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="7"/>
-        <v>165</v>
+        <f t="shared" si="9"/>
+        <v>139</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="7"/>
-        <v>165</v>
+        <f t="shared" si="9"/>
+        <v>139</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="7"/>
-        <v>165</v>
+        <f t="shared" si="9"/>
+        <v>139</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="7"/>
-        <v>165</v>
+        <f t="shared" si="9"/>
+        <v>139</v>
       </c>
       <c r="G5" s="1">
-        <f>A1+9</f>
-        <v>166</v>
+        <f>A1+7</f>
+        <v>140</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H5:L5" si="8">B1+9</f>
-        <v>166</v>
+        <f t="shared" ref="H5:L5" si="10">B1+7</f>
+        <v>140</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="8"/>
-        <v>166</v>
+        <f t="shared" si="10"/>
+        <v>140</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="8"/>
-        <v>166</v>
+        <f t="shared" si="10"/>
+        <v>140</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="8"/>
-        <v>166</v>
+        <f t="shared" si="10"/>
+        <v>140</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="8"/>
-        <v>166</v>
+        <f t="shared" si="10"/>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="199" customHeight="1">
       <c r="A6" s="1">
-        <f t="shared" ref="A6:F6" si="9">A1+9</f>
-        <v>166</v>
+        <f>A1+8</f>
+        <v>141</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="9"/>
-        <v>166</v>
+        <f t="shared" ref="B6:F6" si="11">B1+8</f>
+        <v>141</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="9"/>
-        <v>166</v>
+        <f t="shared" si="11"/>
+        <v>141</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="9"/>
-        <v>166</v>
+        <f t="shared" si="11"/>
+        <v>141</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="9"/>
-        <v>166</v>
+        <f t="shared" si="11"/>
+        <v>141</v>
       </c>
       <c r="F6" s="1">
-        <f>F1+10</f>
-        <v>167</v>
+        <f t="shared" si="11"/>
+        <v>141</v>
       </c>
       <c r="G6" s="1">
-        <f>A1+11</f>
-        <v>168</v>
+        <f>A1+9</f>
+        <v>142</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6:L6" si="10">B1+11</f>
-        <v>168</v>
+        <f t="shared" ref="H6:L6" si="12">B1+9</f>
+        <v>142</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="10"/>
-        <v>168</v>
+        <f t="shared" si="12"/>
+        <v>142</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="10"/>
-        <v>168</v>
+        <f t="shared" si="12"/>
+        <v>142</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="10"/>
-        <v>168</v>
+        <f t="shared" si="12"/>
+        <v>142</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="10"/>
-        <v>168</v>
+        <f t="shared" si="12"/>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="199" customHeight="1">
       <c r="A7" s="1">
-        <v>157</v>
+        <f>A1 +10</f>
+        <v>143</v>
       </c>
       <c r="B7" s="1">
-        <v>157</v>
+        <f>+A7</f>
+        <v>143</v>
       </c>
       <c r="C7" s="1">
-        <v>157</v>
+        <f t="shared" ref="C7:F7" si="13">+B7</f>
+        <v>143</v>
       </c>
       <c r="D7" s="1">
-        <v>157</v>
+        <f t="shared" si="13"/>
+        <v>143</v>
       </c>
       <c r="E7" s="1">
-        <v>157</v>
+        <f t="shared" si="13"/>
+        <v>143</v>
       </c>
       <c r="F7" s="1">
-        <v>157</v>
+        <f t="shared" si="13"/>
+        <v>143</v>
       </c>
       <c r="G7" s="1">
         <f>A7+1</f>
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" ref="H7" si="11">B7+1</f>
-        <v>158</v>
+        <f t="shared" ref="H7:L8" si="14">B7+1</f>
+        <v>144</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" ref="I7" si="12">C7+1</f>
-        <v>158</v>
+        <f t="shared" si="14"/>
+        <v>144</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" ref="J7" si="13">D7+1</f>
-        <v>158</v>
+        <f t="shared" si="14"/>
+        <v>144</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" ref="K7" si="14">E7+1</f>
-        <v>158</v>
+        <f t="shared" si="14"/>
+        <v>144</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7" si="15">F7+1</f>
-        <v>158</v>
+        <f t="shared" si="14"/>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="199" customHeight="1">
       <c r="A8" s="1">
-        <f>A7+2</f>
-        <v>159</v>
+        <f>A1</f>
+        <v>133</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ref="B8" si="16">B7+2</f>
-        <v>159</v>
+        <f>+A8</f>
+        <v>133</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8" si="17">C7+2</f>
-        <v>159</v>
+        <f t="shared" ref="C8:F8" si="15">+B8</f>
+        <v>133</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8" si="18">D7+2</f>
-        <v>159</v>
+        <f t="shared" si="15"/>
+        <v>133</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8" si="19">E7+2</f>
-        <v>159</v>
+        <f t="shared" si="15"/>
+        <v>133</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8" si="20">F7+2</f>
-        <v>159</v>
+        <f t="shared" si="15"/>
+        <v>133</v>
       </c>
       <c r="G8" s="1">
-        <f>A7+3</f>
-        <v>160</v>
+        <f>A8+1</f>
+        <v>134</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ref="H8" si="21">B7+3</f>
-        <v>160</v>
+        <f t="shared" si="14"/>
+        <v>134</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ref="I8" si="22">C7+3</f>
-        <v>160</v>
+        <f t="shared" si="14"/>
+        <v>134</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" ref="J8" si="23">D7+3</f>
-        <v>160</v>
+        <f t="shared" si="14"/>
+        <v>134</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" ref="K8" si="24">E7+3</f>
-        <v>160</v>
+        <f t="shared" si="14"/>
+        <v>134</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" ref="L8" si="25">F7+3</f>
-        <v>160</v>
+        <f t="shared" si="14"/>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="199" customHeight="1">
       <c r="A9" s="1">
-        <f>A7+4</f>
-        <v>161</v>
+        <f>A8+2</f>
+        <v>135</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" ref="B9:F9" si="26">B7+4</f>
-        <v>161</v>
+        <f t="shared" ref="B9" si="16">B8+2</f>
+        <v>135</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="26"/>
-        <v>161</v>
+        <f t="shared" ref="C9" si="17">C8+2</f>
+        <v>135</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="26"/>
-        <v>161</v>
+        <f t="shared" ref="D9" si="18">D8+2</f>
+        <v>135</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="26"/>
-        <v>161</v>
+        <f t="shared" ref="E9" si="19">E8+2</f>
+        <v>135</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="26"/>
-        <v>161</v>
+        <f t="shared" ref="F9" si="20">F8+2</f>
+        <v>135</v>
       </c>
       <c r="G9" s="1">
-        <f>A7+5</f>
-        <v>162</v>
+        <f>A8+3</f>
+        <v>136</v>
       </c>
       <c r="H9" s="1">
-        <v>162</v>
+        <f t="shared" ref="H9" si="21">B8+3</f>
+        <v>136</v>
       </c>
       <c r="I9" s="1">
-        <v>162</v>
+        <f t="shared" ref="I9" si="22">C8+3</f>
+        <v>136</v>
       </c>
       <c r="J9" s="1">
-        <v>162</v>
+        <f t="shared" ref="J9" si="23">D8+3</f>
+        <v>136</v>
       </c>
       <c r="K9" s="1">
-        <v>162</v>
+        <f t="shared" ref="K9" si="24">E8+3</f>
+        <v>136</v>
       </c>
       <c r="L9" s="1">
-        <v>162</v>
+        <f t="shared" ref="L9" si="25">F8+3</f>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="199" customHeight="1">
       <c r="A10" s="1">
-        <f>A7+6</f>
-        <v>163</v>
+        <f>A8+4</f>
+        <v>137</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" ref="B10:F10" si="27">B7+6</f>
-        <v>163</v>
+        <f t="shared" ref="B10:G10" si="26">B8+4</f>
+        <v>137</v>
       </c>
       <c r="C10" s="1">
+        <f t="shared" si="26"/>
+        <v>137</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="26"/>
+        <v>137</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="26"/>
+        <v>137</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="26"/>
+        <v>137</v>
+      </c>
+      <c r="G10" s="1">
+        <f>A8+5</f>
+        <v>138</v>
+      </c>
+      <c r="H10" s="1">
+        <f>B8+5</f>
+        <v>138</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" ref="I10:L10" si="27">C8+5</f>
+        <v>138</v>
+      </c>
+      <c r="J10" s="1">
         <f t="shared" si="27"/>
-        <v>163</v>
-      </c>
-      <c r="D10" s="1">
+        <v>138</v>
+      </c>
+      <c r="K10" s="1">
         <f t="shared" si="27"/>
-        <v>163</v>
-      </c>
-      <c r="E10" s="1">
+        <v>138</v>
+      </c>
+      <c r="L10" s="1">
         <f t="shared" si="27"/>
-        <v>163</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="27"/>
-        <v>163</v>
-      </c>
-      <c r="G10" s="1">
-        <f>A7+7</f>
-        <v>164</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" ref="H10" si="28">B7+7</f>
-        <v>164</v>
-      </c>
-      <c r="I10" s="1">
-        <f t="shared" ref="I10" si="29">C7+7</f>
-        <v>164</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" ref="J10" si="30">D7+7</f>
-        <v>164</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" ref="K10" si="31">E7+7</f>
-        <v>164</v>
-      </c>
-      <c r="L10" s="1">
-        <f t="shared" ref="L10" si="32">F7+7</f>
-        <v>164</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="199" customHeight="1">
       <c r="A11" s="1">
-        <f>A7+8</f>
-        <v>165</v>
+        <f t="shared" ref="A11:B11" si="28">A8+4</f>
+        <v>137</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" ref="B11:F11" si="33">B7+8</f>
-        <v>165</v>
+        <f t="shared" si="28"/>
+        <v>137</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="33"/>
-        <v>165</v>
+        <f>C8+4</f>
+        <v>137</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="33"/>
-        <v>165</v>
+        <f t="shared" ref="D11:F11" si="29">D8+4</f>
+        <v>137</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="33"/>
-        <v>165</v>
+        <f t="shared" si="29"/>
+        <v>137</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="33"/>
-        <v>165</v>
+        <f t="shared" si="29"/>
+        <v>137</v>
       </c>
       <c r="G11" s="1">
-        <f>A7+9</f>
-        <v>166</v>
+        <f>A8+5</f>
+        <v>138</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" ref="H11" si="34">B7+9</f>
-        <v>166</v>
+        <f t="shared" ref="H11" si="30">B8+5</f>
+        <v>138</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" ref="I11" si="35">C7+9</f>
-        <v>166</v>
+        <f t="shared" ref="I11" si="31">C8+5</f>
+        <v>138</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" ref="J11" si="36">D7+9</f>
-        <v>166</v>
+        <f t="shared" ref="J11" si="32">D8+5</f>
+        <v>138</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" ref="K11" si="37">E7+9</f>
-        <v>166</v>
+        <f t="shared" ref="K11" si="33">E8+5</f>
+        <v>138</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" ref="L11" si="38">F7+9</f>
-        <v>166</v>
+        <f t="shared" ref="L11" si="34">F8+5</f>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="199" customHeight="1">
       <c r="A12" s="1">
-        <f t="shared" ref="A12:F12" si="39">A7+9</f>
-        <v>166</v>
+        <f>A8+6</f>
+        <v>139</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="39"/>
-        <v>166</v>
+        <f t="shared" ref="B12:F12" si="35">B8+6</f>
+        <v>139</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="39"/>
-        <v>166</v>
+        <f t="shared" si="35"/>
+        <v>139</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="39"/>
-        <v>166</v>
+        <f t="shared" si="35"/>
+        <v>139</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="39"/>
-        <v>166</v>
+        <f t="shared" si="35"/>
+        <v>139</v>
       </c>
       <c r="F12" s="1">
-        <f>F7+10</f>
-        <v>167</v>
+        <f t="shared" si="35"/>
+        <v>139</v>
       </c>
       <c r="G12" s="1">
-        <f>A7+11</f>
-        <v>168</v>
+        <f>A8+7</f>
+        <v>140</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" ref="H12" si="40">B7+11</f>
-        <v>168</v>
+        <f t="shared" ref="H12" si="36">B8+7</f>
+        <v>140</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" ref="I12" si="41">C7+11</f>
-        <v>168</v>
+        <f t="shared" ref="I12" si="37">C8+7</f>
+        <v>140</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" ref="J12" si="42">D7+11</f>
-        <v>168</v>
+        <f t="shared" ref="J12" si="38">D8+7</f>
+        <v>140</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" ref="K12" si="43">E7+11</f>
-        <v>168</v>
+        <f t="shared" ref="K12" si="39">E8+7</f>
+        <v>140</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" ref="L12" si="44">F7+11</f>
-        <v>168</v>
+        <f t="shared" ref="L12" si="40">F8+7</f>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="199" customHeight="1">
       <c r="A13" s="1">
-        <v>13</v>
+        <f>A8+8</f>
+        <v>141</v>
       </c>
       <c r="B13" s="1">
-        <v>31</v>
+        <f t="shared" ref="B13:F13" si="41">B8+8</f>
+        <v>141</v>
       </c>
       <c r="C13" s="1">
-        <v>49</v>
+        <f t="shared" si="41"/>
+        <v>141</v>
       </c>
       <c r="D13" s="1">
-        <v>67</v>
+        <f t="shared" si="41"/>
+        <v>141</v>
       </c>
       <c r="E13" s="1">
-        <v>85</v>
+        <f t="shared" si="41"/>
+        <v>141</v>
       </c>
       <c r="F13" s="1">
-        <v>103</v>
+        <f t="shared" si="41"/>
+        <v>141</v>
       </c>
       <c r="G13" s="1">
-        <v>121</v>
+        <f>A8+9</f>
+        <v>142</v>
       </c>
       <c r="H13" s="1">
-        <v>139</v>
+        <f t="shared" ref="H13" si="42">B8+9</f>
+        <v>142</v>
       </c>
       <c r="I13" s="1">
-        <v>157</v>
+        <f t="shared" ref="I13" si="43">C8+9</f>
+        <v>142</v>
       </c>
       <c r="J13" s="1">
-        <v>175</v>
+        <f t="shared" ref="J13" si="44">D8+9</f>
+        <v>142</v>
       </c>
       <c r="K13" s="1">
-        <v>193</v>
+        <f t="shared" ref="K13" si="45">E8+9</f>
+        <v>142</v>
       </c>
       <c r="L13" s="1">
-        <v>211</v>
+        <f t="shared" ref="L13" si="46">F8+9</f>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="199" customHeight="1">
       <c r="A14" s="1">
-        <v>14</v>
+        <f>A8 +10</f>
+        <v>143</v>
       </c>
       <c r="B14" s="1">
-        <v>32</v>
+        <f>+A14</f>
+        <v>143</v>
       </c>
       <c r="C14" s="1">
-        <v>50</v>
+        <f t="shared" ref="C14:F14" si="47">+B14</f>
+        <v>143</v>
       </c>
       <c r="D14" s="1">
-        <v>68</v>
+        <f t="shared" si="47"/>
+        <v>143</v>
       </c>
       <c r="E14" s="1">
-        <v>86</v>
+        <f t="shared" si="47"/>
+        <v>143</v>
       </c>
       <c r="F14" s="1">
-        <v>104</v>
+        <f t="shared" si="47"/>
+        <v>143</v>
       </c>
       <c r="G14" s="1">
-        <v>122</v>
+        <f>A14+1</f>
+        <v>144</v>
       </c>
       <c r="H14" s="1">
-        <v>140</v>
+        <f t="shared" ref="H14" si="48">B14+1</f>
+        <v>144</v>
       </c>
       <c r="I14" s="1">
-        <v>158</v>
+        <f t="shared" ref="I14" si="49">C14+1</f>
+        <v>144</v>
       </c>
       <c r="J14" s="1">
-        <v>176</v>
+        <f t="shared" ref="J14" si="50">D14+1</f>
+        <v>144</v>
       </c>
       <c r="K14" s="1">
-        <v>194</v>
+        <f t="shared" ref="K14" si="51">E14+1</f>
+        <v>144</v>
       </c>
       <c r="L14" s="1">
-        <v>212</v>
+        <f t="shared" ref="L14" si="52">F14+1</f>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="199" customHeight="1">
@@ -1248,6 +1288,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="29" fitToHeight="2" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="30" fitToHeight="2" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>